<commit_message>
Finalizado QA. Creado executable con virtual environment prescript-env. Creada requirements.yml final por si hay que hacer enviroment de nuevo. Deshabilitada opcion de abrir con Chrome por no funcionar si el programa se remotea.
</commit_message>
<xml_diff>
--- a/protocols/Protocolo de constraints.xlsx
+++ b/protocols/Protocolo de constraints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9435" tabRatio="895" firstSheet="34" activeTab="44"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9435" tabRatio="895"/>
   </bookViews>
   <sheets>
     <sheet name="NE" sheetId="45" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="166">
   <si>
     <t>Constraint</t>
   </si>
@@ -559,12 +559,15 @@
   <si>
     <t>CBCT una vez por semana + CBCT primeros 3 días representativos para promedios</t>
   </si>
+  <si>
+    <t>NO AGREGAR PESTANAS NUEVAS ANTES DE VMI+BOOST INT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,8 +624,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -716,6 +727,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1045,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1138,6 +1155,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3830,7 +3849,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4094,11 +4113,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="76" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="76" customWidth="1"/>
@@ -4153,7 +4172,9 @@
       <c r="B7" s="89"/>
       <c r="C7" s="89"/>
       <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
+      <c r="E7" s="92" t="s">
+        <v>165</v>
+      </c>
       <c r="F7" s="89"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4253,7 +4274,7 @@
       <c r="B15" s="89"/>
       <c r="C15" s="89"/>
       <c r="D15" s="89"/>
-      <c r="E15" s="90"/>
+      <c r="E15" s="93"/>
       <c r="F15" s="89"/>
       <c r="G15" s="90"/>
       <c r="H15" s="89"/>
@@ -4348,8 +4369,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4361,7 +4382,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -4983,7 +5004,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -5617,7 +5638,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -6270,7 +6291,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -6935,7 +6956,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -7447,7 +7468,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -7971,7 +7992,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -8548,7 +8569,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -9152,7 +9173,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -9738,7 +9759,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -10336,7 +10357,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="76" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="76" customWidth="1"/>
@@ -10590,7 +10611,7 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -11102,7 +11123,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -11626,7 +11647,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -12195,7 +12216,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -12782,7 +12803,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -13371,7 +13392,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -13978,7 +13999,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -14583,7 +14604,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -15257,7 +15278,7 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -15947,7 +15968,7 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -16600,10 +16621,10 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -17084,7 +17105,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -17717,10 +17738,10 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -17917,7 +17938,7 @@
       <c r="A13" s="42"/>
       <c r="B13" s="46"/>
       <c r="C13" s="47" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13" s="46">
         <v>5885</v>
@@ -18351,7 +18372,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -18890,7 +18911,7 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -19580,7 +19601,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -20296,7 +20317,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -20994,7 +21015,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -21692,7 +21713,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -22364,7 +22385,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -22862,7 +22883,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -23360,7 +23381,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -23777,7 +23798,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -24315,7 +24336,7 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -24892,11 +24913,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -25031,9 +25052,7 @@
       <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="77"/>
       <c r="D10" s="43"/>
@@ -25374,11 +25393,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -25513,9 +25532,7 @@
       <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="77"/>
       <c r="D10" s="43"/>
@@ -25857,10 +25874,10 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -25995,9 +26012,7 @@
       <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="77"/>
       <c r="D10" s="43"/>
@@ -26341,11 +26356,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -26480,9 +26495,7 @@
       <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="77"/>
       <c r="D10" s="43"/>
@@ -26830,7 +26843,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -27263,7 +27276,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -27890,7 +27903,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -28533,7 +28546,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>
@@ -29115,7 +29128,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="30.7109375" style="76" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" style="76" customWidth="1"/>

</xml_diff>